<commit_message>
fix parsing no name
</commit_message>
<xml_diff>
--- a/Book2 Uji coba secrip config (1).xlsx
+++ b/Book2 Uji coba secrip config (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ngoprek2\2024\mikolt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FFC33D-F82A-4EE7-85C6-B57E77ADD3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C67A0-C771-4EDB-9C16-64A097ECE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BD51175B-3152-4DA7-BEF2-AAF7E076EA07}"/>
+    <workbookView xWindow="34680" yWindow="3720" windowWidth="17280" windowHeight="8880" xr2:uid="{BD51175B-3152-4DA7-BEF2-AAF7E076EA07}"/>
   </bookViews>
   <sheets>
     <sheet name="KCM" sheetId="1" r:id="rId1"/>
@@ -762,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CFCCA8-08C6-4B86-B1B5-4A5D9A1A8F31}">
   <dimension ref="B1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>